<commit_message>
fix bug that auto flat arr in some case
</commit_message>
<xml_diff>
--- a/test/demo.xlsx
+++ b/test/demo.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12040" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="12080" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91">
   <si>
     <t>No</t>
   </si>
@@ -181,6 +183,114 @@
   </si>
   <si>
     <t>[10000, 99999999999)</t>
+  </si>
+  <si>
+    <t>1~1</t>
+  </si>
+  <si>
+    <t>1~2</t>
+  </si>
+  <si>
+    <t>2~1</t>
+  </si>
+  <si>
+    <t>2~2</t>
+  </si>
+  <si>
+    <t>3~1</t>
+  </si>
+  <si>
+    <t>3~2</t>
+  </si>
+  <si>
+    <t>1~3</t>
+  </si>
+  <si>
+    <t>1~4</t>
+  </si>
+  <si>
+    <t>2~3</t>
+  </si>
+  <si>
+    <t>2~4</t>
+  </si>
+  <si>
+    <t>3~3</t>
+  </si>
+  <si>
+    <t>3~4</t>
+  </si>
+  <si>
+    <t>4~1</t>
+  </si>
+  <si>
+    <t>4~2</t>
+  </si>
+  <si>
+    <t>5~1</t>
+  </si>
+  <si>
+    <t>5~2</t>
+  </si>
+  <si>
+    <t>6~1</t>
+  </si>
+  <si>
+    <t>6~2</t>
+  </si>
+  <si>
+    <t>4~3</t>
+  </si>
+  <si>
+    <t>4~4</t>
+  </si>
+  <si>
+    <t>5~3</t>
+  </si>
+  <si>
+    <t>5~4</t>
+  </si>
+  <si>
+    <t>6~3</t>
+  </si>
+  <si>
+    <t>6~4</t>
+  </si>
+  <si>
+    <t>7~1</t>
+  </si>
+  <si>
+    <t>7~2</t>
+  </si>
+  <si>
+    <t>8~1</t>
+  </si>
+  <si>
+    <t>8~2</t>
+  </si>
+  <si>
+    <t>9~1</t>
+  </si>
+  <si>
+    <t>9~2</t>
+  </si>
+  <si>
+    <t>7~3</t>
+  </si>
+  <si>
+    <t>7~4</t>
+  </si>
+  <si>
+    <t>8~3</t>
+  </si>
+  <si>
+    <t>8~4</t>
+  </si>
+  <si>
+    <t>9~3</t>
+  </si>
+  <si>
+    <t>9~4</t>
   </si>
 </sst>
 </file>
@@ -189,10 +299,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -218,6 +328,67 @@
       <color rgb="FF333333"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -229,8 +400,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -244,66 +432,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -313,17 +441,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -334,36 +454,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -386,97 +496,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -488,73 +658,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -565,6 +675,41 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -593,6 +738,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -607,32 +767,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -641,182 +775,161 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -1156,268 +1269,268 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:H10"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="7"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="5">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="6">
         <v>32</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="8">
         <v>42948</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="6">
         <v>1562</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="5">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="6">
         <v>25</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="8">
         <v>42949</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="6">
         <v>1582</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="5">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="6">
         <v>36</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="8">
         <v>42950</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="6">
         <v>2587</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="5">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="6">
         <v>25</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="8">
         <v>42951</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="6">
         <v>3549</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="5">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="6">
         <v>58</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="8">
         <v>42952</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="6">
         <v>2468</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="5">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="6">
         <v>24</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="8">
         <v>42953</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="6">
         <v>2554</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="5">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="6">
         <v>56</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="8">
         <v>42954</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="6">
         <v>3598</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="5">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="6">
         <v>27</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="8">
         <v>42955</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="6">
         <v>2456</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="5">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="6">
         <v>40</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="8">
         <v>42956</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="6">
         <v>6548</v>
       </c>
     </row>
@@ -1439,23 +1552,23 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="5">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
@@ -1469,81 +1582,81 @@
       </c>
     </row>
     <row r="3" ht="14.8" spans="1:5">
-      <c r="A3" s="5">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" ht="14.8" spans="1:5">
-      <c r="A4" s="5">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" ht="14.8" spans="1:5">
-      <c r="A5" s="5">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="6" ht="14.8" spans="1:5">
-      <c r="A6" s="5">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="7" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="7" ht="14.8" spans="1:5">
-      <c r="A7" s="5">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>48</v>
       </c>
       <c r="D7" t="s">
@@ -1554,53 +1667,53 @@
       </c>
     </row>
     <row r="8" ht="14.8" spans="1:5">
-      <c r="A8" s="5">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="9" ht="14.8" spans="1:5">
-      <c r="A9" s="5">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="10" ht="14.8" spans="1:5">
-      <c r="A10" s="5">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="7" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1618,8 +1731,8 @@
   <sheetPr/>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="1"/>
@@ -1640,7 +1753,7 @@
       <c r="A2" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1648,7 +1761,7 @@
       <c r="A3" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>0.2</v>
       </c>
     </row>
@@ -1656,7 +1769,7 @@
       <c r="A4" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>0.4</v>
       </c>
     </row>
@@ -1664,8 +1777,288 @@
       <c r="A5" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>0.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="5" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="7"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>